<commit_message>
Add all field search
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zolttoth/ElasticSample/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zolttoth/ElasticsearchDemo/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>production_id</t>
   </si>
@@ -62,25 +62,7 @@
     <t>asset77777</t>
   </si>
   <si>
-    <t>asset88888</t>
-  </si>
-  <si>
     <t>asset99999</t>
-  </si>
-  <si>
-    <t>Mauris enim ex, tempus non lectus vestibulum, malesuada semper enim. Pellentesque ante ante, dignissim quis lectus nec, volutpat condimentum diam. Nunc non nisl vel est commodo tempus. Pellentesque placerat, libero quis auctor cursus, mauris enim dapibus mi, vulputate faucibus velit eros at nunc. Pellentesque sit amet malesuada purus, dignissim posuere erat. Cras hendrerit luctus vestibulum. Nullam imperdiet sapien nec ligula sagittis mollis vel in velit. Nunc euismod erat felis, sit amet dignissim ligula consequat ut. Nullam eget magna eros. Suspendisse imperdiet, est quis iaculis volutpat, leo nisl laoreet arcu, at tincidunt nisi nunc eu felis. Cras euismod auctor ipsum a gravida. Donec pulvinar nisl ac purus varius vehicula. Fusce vitae nunc egestas, tincidunt ante quis, rhoncus massa. Proin laoreet pretium sapien id vehicula. Nunc in finibus purus, ut maximus odio. Nunc eu laoreet lectus.</t>
-  </si>
-  <si>
-    <t>Nulla euismod arcu quam, vitae lacinia lacus elementum et. Aliquam elit erat, auctor volutpat eros ac, mattis imperdiet est. Aliquam erat volutpat. Ut eget erat vel lectus luctus ullamcorper ut a odio. Donec ultricies viverra nibh, quis rhoncus ante dictum vel. Lorem ipsum dolor sit amet, consectetur adipiscing elit. Sed viverra euismod rhoncus. Vestibulum elementum et ipsum at volutpat. Phasellus eu est eu urna mattis cursus. Curabitur est tortor, luctus vitae efficitur eu, ornare non lacus. Praesent nec mi mollis quam porta ullamcorper sit amet at tellus.</t>
-  </si>
-  <si>
-    <t>Pellentesque hendrerit mi consectetur augue ullamcorper varius. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Donec ut dignissim justo, eget rhoncus urna. Aliquam eu ipsum augue. Nam tempor sollicitudin ex. Morbi pellentesque lacus ut nisl commodo porta. Pellentesque porttitor, nulla nec posuere efficitur, dui risus vestibulum augue, sed cursus ipsum nisl in justo. Nunc finibus lorem id mauris rutrum eleifend.</t>
-  </si>
-  <si>
-    <t>Aliquam non faucibus nibh. Duis dictum ipsum eget sem dictum tempor. Duis elementum tincidunt vestibulum. Fusce ante ante, faucibus sit amet lectus id, tincidunt tincidunt purus. Nam aliquam porta mi. Nulla facilisi. Sed semper auctor dictum. Curabitur auctor, orci sed finibus ullamcorper, odio arcu blandit purus, id scelerisque enim nibh nec ante. Nullam cursus nibh id nunc mollis molestie. Duis velit eros, varius dignissim scelerisque ut, imperdiet nec nibh. Quisque varius neque eget est gravida, sed pulvinar risus sodales.</t>
-  </si>
-  <si>
-    <t>Sed sed sapien at erat malesuada lobortis quis ac enim. Morbi nisl dolor, malesuada ac arcu at, varius vulputate mauris. Maecenas tincidunt enim orci, sed viverra nisl aliquam sit amet. Aliquam in diam nec justo blandit hendrerit. Vivamus ac dapibus nibh. Proin et mi vel lorem congue viverra. Nunc non mollis nisi. Etiam porta ante at maximus molestie. Morbi convallis vel sapien vitae gravida. Vivamus diam libero, tincidunt sit amet rhoncus vel, porta sit amet justo. Donec vestibulum ornare accumsan. Nulla vel magna finibus sapien sodales maximus et ut lacus. Praesent nunc odio, aliquam eu ex eu, tempus luctus est. Sed non ullamcorper tortor, a condimentum felis. Suspendisse sodales, quam sit amet sagittis vehicula, nisi massa blandit ante, convallis consectetur diam leo in nunc. Mauris sapien sapien, efficitur ut ullamcorper ac, consequat eget felis.</t>
   </si>
   <si>
     <t>Pellentesque odio libero, malesuada id elit et,  David tempor accumsan nisi. Aenean commodo elementum justo, in molestie erat aliquam a. Cras nec elit nisl. Ut elit nibh, consectetur non quam a, suscipit facilisis dui. Maecenas tincidunt, leo quis placerat interdum, nunc risus placerat lacus, convallis sodales odio mauris sit amet magna. Praesent auctor dui sapien, fringilla feugiat dolor malesuada sit amet. Nulla fermentum mattis ante facilisis placerat. Mauris orci sapien, facilisis eu dignissim at, iaculis in massa. Curabitur blandit efficitur rutrum. Vestibulum at sem id ante molestie facilisis. Morbi rutrum, augue quis facilisis pellentesque, velit lorem fringilla odio, nec dapibus lorem ipsum ut felis. Aliquam bibendum finibus libero, ut cursus justo commodo id. Phasellus eget mi eu turpis convallis blandit. Praesent gravida vulputate velit, vel condimentum est viverra ac.</t>
@@ -154,6 +136,21 @@
   </si>
   <si>
     <t>4tret43t45t55</t>
+  </si>
+  <si>
+    <t>Brown fox brown dog</t>
+  </si>
+  <si>
+    <t>The quick brown fox jumps over the lazy dog</t>
+  </si>
+  <si>
+    <t>The quick brown fox jumps over the quick dog</t>
+  </si>
+  <si>
+    <t>Tzoli</t>
+  </si>
+  <si>
+    <t>dffefewfew</t>
   </si>
 </sst>
 </file>
@@ -481,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,13 +513,13 @@
         <v>11111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -533,13 +530,13 @@
         <v>22222</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="288" x14ac:dyDescent="0.2">
@@ -553,7 +550,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="224" x14ac:dyDescent="0.2">
@@ -564,16 +561,16 @@
         <v>44444</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="304" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>222</v>
       </c>
@@ -584,10 +581,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>222</v>
       </c>
@@ -595,16 +592,16 @@
         <v>66666</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>333</v>
       </c>
@@ -615,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>333</v>
       </c>
@@ -626,13 +623,13 @@
         <v>88888</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="288" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>333</v>
       </c>
@@ -640,13 +637,13 @@
         <v>99999</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>